<commit_message>
Adding test case 702
</commit_message>
<xml_diff>
--- a/test_files/Modify_dpm_metric.xlsx
+++ b/test_files/Modify_dpm_metric.xlsx
@@ -17,6 +17,84 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="200">
   <si>
+    <t>HREF</t>
+  </si>
+  <si>
+    <t>PROPERTYTYPE</t>
+  </si>
+  <si>
+    <t>TITLE_FI</t>
+  </si>
+  <si>
+    <t>TITLE_SV</t>
+  </si>
+  <si>
+    <t>TITLE_EN</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_FI</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>CREATED</t>
+  </si>
+  <si>
+    <t>MODIFIED</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>Creative Commons Nimeä 4.0 Kansainvälinen (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons Erkännande 4.0 Internationell (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons Attribution 4.0 International (CC BY 4.0)</t>
+  </si>
+  <si>
+    <t>Koodisto on lisensoitu Creative Commons Nimeä 4.0 Kansainvälinen -lisenssillä.</t>
+  </si>
+  <si>
+    <t>Detta kodelist är licensierat under en Creative Commons Erkännande 4.0 Internationell Licens.</t>
+  </si>
+  <si>
+    <t>This code list is licensed under a Creative Commons Attribution 4.0 International License.</t>
+  </si>
+  <si>
+    <t>2018-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
+  </si>
+  <si>
+    <t>Creative Commons CC0 1.0 Yleismaailmallinen (CC0 1.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons CC0 1.0 universell (CC0 1.0)</t>
+  </si>
+  <si>
+    <t>Creative Commons CC0 1.0 Universal (CC0 1.0)</t>
+  </si>
+  <si>
+    <t>Koodisto on lisensoitu Creative Commons Zero (CC0) -lisenssillä.</t>
+  </si>
+  <si>
+    <t>Detta kodelist är licensierat under en Creative Commons Zero (CC0) Licens.</t>
+  </si>
+  <si>
+    <t>This code list is licensed under a Creative Commons Zero (CC0) License.</t>
+  </si>
+  <si>
     <t>CODEVALUE</t>
   </si>
   <si>
@@ -32,25 +110,37 @@
     <t>VERSION</t>
   </si>
   <si>
+    <t>BROADER</t>
+  </si>
+  <si>
     <t>STATUS</t>
   </si>
   <si>
     <t>SOURCE</t>
   </si>
   <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
     <t>LEGALBASE</t>
   </si>
   <si>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
     <t>GOVERNANCEPOLICY</t>
   </si>
   <si>
     <t>CONCEPTURI</t>
   </si>
   <si>
+    <t>HIERARCHYLEVEL</t>
+  </si>
+  <si>
     <t>DEFAULTCODE</t>
   </si>
   <si>
-    <t>PREFLABEL_FI</t>
+    <t>ORDER</t>
   </si>
   <si>
     <t>STARTDATE</t>
@@ -59,15 +149,6 @@
     <t>ENDDATE</t>
   </si>
   <si>
-    <t>CREATED</t>
-  </si>
-  <si>
-    <t>MODIFIED</t>
-  </si>
-  <si>
-    <t>HREF</t>
-  </si>
-  <si>
     <t>CODESSHEET</t>
   </si>
   <si>
@@ -77,91 +158,34 @@
     <t>EXTENSIONSSHEET</t>
   </si>
   <si>
-    <t>BROADER</t>
-  </si>
-  <si>
-    <t>PROPERTYTYPE</t>
-  </si>
-  <si>
-    <t>TITLE_FI</t>
-  </si>
-  <si>
-    <t>TITLE_SV</t>
-  </si>
-  <si>
-    <t>TITLE_EN</t>
-  </si>
-  <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>HIERARCHYLEVEL</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>ORDER</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by/4.0/</t>
-  </si>
-  <si>
     <t>testcode28</t>
   </si>
   <si>
-    <t>license</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>600</t>
   </si>
   <si>
-    <t>Creative Commons Nimeä 4.0 Kansainvälinen (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>Creative Commons Erkännande 4.0 Internationell (CC BY 4.0)</t>
+    <t>DRAFT</t>
   </si>
   <si>
     <t>74a41211-8c99-4835-a519-7a61612b1098</t>
   </si>
   <si>
-    <t>Creative Commons Attribution 4.0 International (CC BY 4.0)</t>
-  </si>
-  <si>
-    <t>DRAFT</t>
+    <t>Testcode 28</t>
   </si>
   <si>
     <t>P1</t>
   </si>
   <si>
-    <t>Testcode 28</t>
-  </si>
-  <si>
     <t>en;fi</t>
   </si>
   <si>
-    <t>Koodisto on lisensoitu Creative Commons Nimeä 4.0 Kansainvälinen -lisenssillä.</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Detta kodelist är licensierat under en Creative Commons Erkännande 4.0 Internationell Licens.</t>
-  </si>
-  <si>
-    <t>This code list is licensed under a Creative Commons Attribution 4.0 International License.</t>
-  </si>
-  <si>
-    <t>2018-01-01 00:00:00</t>
+    <t>testcode29</t>
   </si>
   <si>
     <t>Koodisto600</t>
@@ -170,45 +194,21 @@
     <t>2018-01-01</t>
   </si>
   <si>
-    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
-  </si>
-  <si>
     <t>2019-01-01</t>
   </si>
   <si>
+    <t>Testcode 29</t>
+  </si>
+  <si>
     <t>Codes_600</t>
   </si>
   <si>
-    <t>Creative Commons CC0 1.0 Yleismaailmallinen (CC0 1.0)</t>
-  </si>
-  <si>
     <t>Links_600</t>
   </si>
   <si>
-    <t>Creative Commons CC0 1.0 universell (CC0 1.0)</t>
-  </si>
-  <si>
-    <t>Creative Commons CC0 1.0 Universal (CC0 1.0)</t>
-  </si>
-  <si>
     <t>Extensions_600</t>
   </si>
   <si>
-    <t>Koodisto on lisensoitu Creative Commons Zero (CC0) -lisenssillä.</t>
-  </si>
-  <si>
-    <t>Detta kodelist är licensierat under en Creative Commons Zero (CC0) Licens.</t>
-  </si>
-  <si>
-    <t>This code list is licensed under a Creative Commons Zero (CC0) License.</t>
-  </si>
-  <si>
-    <t>testcode29</t>
-  </si>
-  <si>
-    <t>Testcode 29</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -470,19 +470,40 @@
     <t>DPMDOMAINREFERENCE</t>
   </si>
   <si>
+    <t>DPMHIERARCHYREFERENCE</t>
+  </si>
+  <si>
     <t>CODESCHEMES</t>
   </si>
   <si>
-    <t>DPMHIERARCHYREFERENCE</t>
-  </si>
-  <si>
     <t>DPMBALANCETYPE</t>
   </si>
   <si>
+    <t>DPMMETRICDATATYPE</t>
+  </si>
+  <si>
     <t>PREFLABEL_EN</t>
   </si>
   <si>
-    <t>DPMDATATYPE</t>
+    <t>MEMBERSSHEET</t>
+  </si>
+  <si>
+    <t>dpmMetric</t>
+  </si>
+  <si>
+    <t>DPM Metric laajennus</t>
+  </si>
+  <si>
+    <t>DPM Metric</t>
+  </si>
+  <si>
+    <t>2018-11-01</t>
+  </si>
+  <si>
+    <t>2020-11-01</t>
+  </si>
+  <si>
+    <t>Members_600_dpmMetric</t>
   </si>
   <si>
     <t>CODE</t>
@@ -491,28 +512,7 @@
     <t>RELATION</t>
   </si>
   <si>
-    <t>MEMBERSSHEET</t>
-  </si>
-  <si>
-    <t>dpmMetric</t>
-  </si>
-  <si>
-    <t>DPM Metric laajennus</t>
-  </si>
-  <si>
-    <t>DPM Metric</t>
-  </si>
-  <si>
-    <t>2018-11-01</t>
-  </si>
-  <si>
-    <t>2020-11-01</t>
-  </si>
-  <si>
     <t>ddd</t>
-  </si>
-  <si>
-    <t>Members_600_dpmMetric</t>
   </si>
   <si>
     <t>ccc</t>
@@ -624,12 +624,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
@@ -655,13 +656,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -709,125 +711,124 @@
     <col customWidth="1" min="15" max="17" width="8.71"/>
     <col customWidth="1" min="18" max="19" width="17.14"/>
     <col customWidth="1" min="20" max="20" width="18.0"/>
-    <col customWidth="1" min="21" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="R2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1828,103 +1829,103 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="8.71"/>
+    <col customWidth="1" min="1" max="10" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2930,118 +2931,118 @@
     <col customWidth="1" min="3" max="10" width="8.71"/>
     <col customWidth="1" min="11" max="11" width="20.29"/>
     <col customWidth="1" min="12" max="12" width="22.86"/>
-    <col customWidth="1" min="13" max="25" width="8.71"/>
+    <col customWidth="1" min="13" max="13" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
         <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -3049,34 +3050,34 @@
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
         <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -3084,34 +3085,34 @@
         <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
         <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
@@ -3119,34 +3120,34 @@
         <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
         <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -3154,34 +3155,34 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
         <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
@@ -3189,34 +3190,34 @@
         <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
         <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -3224,34 +3225,34 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -3259,34 +3260,34 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
         <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
@@ -3294,34 +3295,34 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
         <v>88</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -3329,34 +3330,34 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
         <v>91</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -3364,34 +3365,34 @@
         <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
         <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
         <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -3399,34 +3400,34 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
         <v>97</v>
       </c>
       <c r="I14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
@@ -3434,34 +3435,34 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
         <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M15" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -3469,34 +3470,34 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
         <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M16" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
@@ -3504,34 +3505,34 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
         <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
         <v>106</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M17" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -3539,34 +3540,34 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
         <v>109</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19">
@@ -3574,34 +3575,34 @@
         <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
         <v>112</v>
       </c>
       <c r="I19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M19" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
@@ -3609,34 +3610,34 @@
         <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
         <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
         <v>115</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M20" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -3644,34 +3645,34 @@
         <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
         <v>118</v>
       </c>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M21" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -3679,34 +3680,34 @@
         <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
         <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
         <v>121</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -3714,34 +3715,34 @@
         <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H23" t="s">
         <v>124</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -3749,34 +3750,34 @@
         <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>127</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M24" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -3784,34 +3785,34 @@
         <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>129</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
         <v>130</v>
       </c>
       <c r="I25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -3819,34 +3820,34 @@
         <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
         <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H26" t="s">
         <v>133</v>
       </c>
       <c r="I26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M26" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -3854,34 +3855,34 @@
         <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H27" t="s">
         <v>136</v>
       </c>
       <c r="I27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M27" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -3889,34 +3890,34 @@
         <v>137</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
         <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H28" t="s">
         <v>139</v>
       </c>
       <c r="I28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M28" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -3924,34 +3925,34 @@
         <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G29" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
         <v>142</v>
       </c>
       <c r="I29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M29" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -3959,34 +3960,34 @@
         <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
         <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H30" t="s">
         <v>145</v>
       </c>
       <c r="I30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -3994,34 +3995,34 @@
         <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
         <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G31" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H31" t="s">
         <v>148</v>
       </c>
       <c r="I31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="M31" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
@@ -5022,71 +5023,70 @@
     <col customWidth="1" min="9" max="9" width="12.57"/>
     <col customWidth="1" min="10" max="10" width="18.86"/>
     <col customWidth="1" min="11" max="11" width="26.86"/>
-    <col customWidth="1" min="12" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" t="s">
         <v>159</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>160</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>161</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>162</v>
-      </c>
-      <c r="H2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6098,7 +6098,7 @@
     <col customWidth="1" min="9" max="9" width="24.43"/>
     <col customWidth="1" min="10" max="10" width="21.14"/>
     <col customWidth="1" min="11" max="11" width="18.86"/>
-    <col customWidth="1" min="12" max="25" width="8.71"/>
+    <col customWidth="1" min="12" max="12" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6109,39 +6109,39 @@
         <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
         <v>153</v>
       </c>
-      <c r="E1" t="s">
-        <v>155</v>
+      <c r="E1" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>166</v>
@@ -6159,18 +6159,18 @@
         <v>170</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2">
         <v>43101.0</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>43831.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
         <v>166</v>
@@ -6187,16 +6187,16 @@
       <c r="F3" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>43102.0</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>43832.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>166</v>
@@ -6213,16 +6213,16 @@
       <c r="F4" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>43103.0</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>43833.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>166</v>
@@ -6239,16 +6239,16 @@
       <c r="F5" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>43104.0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>43834.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>166</v>
@@ -6265,16 +6265,16 @@
       <c r="F6" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>43105.0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>43835.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>166</v>
@@ -6291,16 +6291,16 @@
       <c r="F7" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>43106.0</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>43836.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>166</v>
@@ -6317,16 +6317,16 @@
       <c r="F8" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>43107.0</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>43837.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>166</v>
@@ -6343,16 +6343,16 @@
       <c r="F9" t="s">
         <v>177</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>43108.0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>43838.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>166</v>
@@ -6369,16 +6369,16 @@
       <c r="F10" t="s">
         <v>178</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>43109.0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2">
         <v>43839.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>166</v>
@@ -6395,16 +6395,16 @@
       <c r="F11" t="s">
         <v>179</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>43110.0</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>43840.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
         <v>166</v>
@@ -6421,16 +6421,16 @@
       <c r="F12" t="s">
         <v>180</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>43111.0</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>43841.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>166</v>
@@ -6447,16 +6447,16 @@
       <c r="F13" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>43112.0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2">
         <v>43842.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
         <v>166</v>
@@ -6473,16 +6473,16 @@
       <c r="F14" t="s">
         <v>182</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>43113.0</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="2">
         <v>43843.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>166</v>
@@ -6499,16 +6499,16 @@
       <c r="F15" t="s">
         <v>183</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>43114.0</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2">
         <v>43844.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
         <v>166</v>
@@ -6525,16 +6525,16 @@
       <c r="F16" t="s">
         <v>184</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>43115.0</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="2">
         <v>43845.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
         <v>166</v>
@@ -6551,16 +6551,16 @@
       <c r="F17" t="s">
         <v>185</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>43116.0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="2">
         <v>43846.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
         <v>166</v>
@@ -6577,16 +6577,16 @@
       <c r="F18" t="s">
         <v>186</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>43117.0</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="2">
         <v>43847.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
         <v>166</v>
@@ -6603,16 +6603,16 @@
       <c r="F19" t="s">
         <v>187</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>43118.0</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="2">
         <v>43848.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
         <v>166</v>
@@ -6629,16 +6629,16 @@
       <c r="F20" t="s">
         <v>188</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>43119.0</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="2">
         <v>43849.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
         <v>166</v>
@@ -6655,16 +6655,16 @@
       <c r="F21" t="s">
         <v>189</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>43120.0</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="2">
         <v>43850.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
         <v>166</v>
@@ -6681,16 +6681,16 @@
       <c r="F22" t="s">
         <v>190</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>43121.0</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="2">
         <v>43851.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
         <v>166</v>
@@ -6707,16 +6707,16 @@
       <c r="F23" t="s">
         <v>191</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <v>43122.0</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="2">
         <v>43852.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B24" t="s">
         <v>166</v>
@@ -6733,16 +6733,16 @@
       <c r="F24" t="s">
         <v>192</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <v>43123.0</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="2">
         <v>43853.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
         <v>166</v>
@@ -6759,16 +6759,16 @@
       <c r="F25" t="s">
         <v>193</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <v>43124.0</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="2">
         <v>43854.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
         <v>166</v>
@@ -6785,16 +6785,16 @@
       <c r="F26" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <v>43125.0</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="2">
         <v>43855.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B27" t="s">
         <v>166</v>
@@ -6811,16 +6811,16 @@
       <c r="F27" t="s">
         <v>195</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <v>43126.0</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="2">
         <v>43856.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
         <v>166</v>
@@ -6837,16 +6837,16 @@
       <c r="F28" t="s">
         <v>196</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>43127.0</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="2">
         <v>43857.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
         <v>166</v>
@@ -6863,16 +6863,16 @@
       <c r="F29" t="s">
         <v>197</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <v>43128.0</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="2">
         <v>43858.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
         <v>166</v>
@@ -6889,16 +6889,16 @@
       <c r="F30" t="s">
         <v>198</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="2">
         <v>43129.0</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="2">
         <v>43859.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
         <v>166</v>
@@ -6915,10 +6915,10 @@
       <c r="F31" t="s">
         <v>199</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="2">
         <v>43130.0</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="2">
         <v>43860.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Extension values corrected
</commit_message>
<xml_diff>
--- a/test_files/Modify_dpm_metric.xlsx
+++ b/test_files/Modify_dpm_metric.xlsx
@@ -15,11 +15,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="211">
+  <si>
+    <t>CODEVALUE</t>
+  </si>
+  <si>
+    <t>BROADER</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>PREFLABEL_FI</t>
+  </si>
+  <si>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
+    <t>CONCEPTURI</t>
+  </si>
+  <si>
+    <t>HIERARCHYLEVEL</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>CREATED</t>
+  </si>
+  <si>
+    <t>MODIFIED</t>
+  </si>
   <si>
     <t>HREF</t>
   </si>
   <si>
+    <t>testcode28</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
+    <t>Testcode 28</t>
+  </si>
+  <si>
     <t>PROPERTYTYPE</t>
   </si>
   <si>
@@ -41,15 +89,45 @@
     <t>DESCRIPTION_EN</t>
   </si>
   <si>
-    <t>CREATED</t>
-  </si>
-  <si>
-    <t>MODIFIED</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>testcode29</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>INFORMATIONDOMAIN</t>
+  </si>
+  <si>
+    <t>LANGUAGECODE</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>LEGALBASE</t>
+  </si>
+  <si>
+    <t>GOVERNANCEPOLICY</t>
+  </si>
+  <si>
+    <t>DEFAULTCODE</t>
+  </si>
+  <si>
+    <t>Testcode 29</t>
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>license</t>
   </si>
   <si>
@@ -59,30 +137,93 @@
     <t>Creative Commons Erkännande 4.0 Internationell (CC BY 4.0)</t>
   </si>
   <si>
+    <t>CODESSHEET</t>
+  </si>
+  <si>
+    <t>testcode30</t>
+  </si>
+  <si>
+    <t>LINKSSHEET</t>
+  </si>
+  <si>
     <t>Creative Commons Attribution 4.0 International (CC BY 4.0)</t>
   </si>
   <si>
+    <t>EXTENSIONSSHEET</t>
+  </si>
+  <si>
+    <t>Testcode 30</t>
+  </si>
+  <si>
     <t>Koodisto on lisensoitu Creative Commons Nimeä 4.0 Kansainvälinen -lisenssillä.</t>
   </si>
   <si>
     <t>Detta kodelist är licensierat under en Creative Commons Erkännande 4.0 Internationell Licens.</t>
   </si>
   <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>en;fi</t>
+  </si>
+  <si>
     <t>This code list is licensed under a Creative Commons Attribution 4.0 International License.</t>
   </si>
   <si>
+    <t>testcode31</t>
+  </si>
+  <si>
     <t>2018-01-01 00:00:00</t>
   </si>
   <si>
+    <t>Testcode 31</t>
+  </si>
+  <si>
+    <t>Koodisto600</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
   </si>
   <si>
+    <t>Codes_600</t>
+  </si>
+  <si>
+    <t>Links_600</t>
+  </si>
+  <si>
+    <t>Extensions_600</t>
+  </si>
+  <si>
     <t>Creative Commons CC0 1.0 Yleismaailmallinen (CC0 1.0)</t>
   </si>
   <si>
+    <t>testcode32</t>
+  </si>
+  <si>
     <t>Creative Commons CC0 1.0 universell (CC0 1.0)</t>
   </si>
   <si>
+    <t>Testcode 32</t>
+  </si>
+  <si>
     <t>Creative Commons CC0 1.0 Universal (CC0 1.0)</t>
   </si>
   <si>
@@ -92,153 +233,12 @@
     <t>Detta kodelist är licensierat under en Creative Commons Zero (CC0) Licens.</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>This code list is licensed under a Creative Commons Zero (CC0) License.</t>
   </si>
   <si>
-    <t>CODEVALUE</t>
-  </si>
-  <si>
-    <t>ORGANIZATION</t>
-  </si>
-  <si>
-    <t>INFORMATIONDOMAIN</t>
-  </si>
-  <si>
-    <t>LANGUAGECODE</t>
-  </si>
-  <si>
-    <t>VERSION</t>
-  </si>
-  <si>
-    <t>BROADER</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
-    <t>PREFLABEL_FI</t>
-  </si>
-  <si>
-    <t>LEGALBASE</t>
-  </si>
-  <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>GOVERNANCEPOLICY</t>
-  </si>
-  <si>
-    <t>CONCEPTURI</t>
-  </si>
-  <si>
-    <t>HIERARCHYLEVEL</t>
-  </si>
-  <si>
-    <t>DEFAULTCODE</t>
-  </si>
-  <si>
-    <t>ORDER</t>
-  </si>
-  <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
-    <t>CODESSHEET</t>
-  </si>
-  <si>
-    <t>LINKSSHEET</t>
-  </si>
-  <si>
-    <t>EXTENSIONSSHEET</t>
-  </si>
-  <si>
-    <t>testcode28</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>DRAFT</t>
-  </si>
-  <si>
-    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
-  </si>
-  <si>
-    <t>Testcode 28</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>en;fi</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>testcode29</t>
-  </si>
-  <si>
-    <t>Koodisto600</t>
-  </si>
-  <si>
-    <t>2018-01-01</t>
-  </si>
-  <si>
-    <t>2019-01-01</t>
-  </si>
-  <si>
-    <t>Testcode 29</t>
-  </si>
-  <si>
-    <t>Codes_600</t>
-  </si>
-  <si>
-    <t>Links_600</t>
-  </si>
-  <si>
-    <t>Extensions_600</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>testcode30</t>
-  </si>
-  <si>
-    <t>Testcode 30</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>testcode31</t>
-  </si>
-  <si>
-    <t>Testcode 31</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>testcode32</t>
-  </si>
-  <si>
-    <t>Testcode 32</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>testcode33</t>
   </si>
   <si>
@@ -485,9 +485,18 @@
     <t>PREFLABEL_EN</t>
   </si>
   <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>RELATION</t>
+  </si>
+  <si>
     <t>MEMBERSSHEET</t>
   </si>
   <si>
+    <t>Instant</t>
+  </si>
+  <si>
     <t>dpmMetric</t>
   </si>
   <si>
@@ -506,25 +515,16 @@
     <t>Members_600_dpmMetric</t>
   </si>
   <si>
-    <t>CODE</t>
-  </si>
-  <si>
-    <t>RELATION</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
     <t>ccc</t>
   </si>
   <si>
     <t>eee</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Enumeration</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode28</t>
@@ -545,6 +545,9 @@
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode33</t>
   </si>
   <si>
+    <t>Boolean</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode34</t>
   </si>
   <si>
@@ -560,24 +563,39 @@
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode38</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode39</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode40</t>
   </si>
   <si>
+    <t>Integer</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode41</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode42</t>
   </si>
   <si>
+    <t>Duration</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode43</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode44</t>
   </si>
   <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Monetary</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode45</t>
   </si>
   <si>
@@ -587,6 +605,9 @@
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode47</t>
   </si>
   <si>
+    <t>Percentage</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode48</t>
   </si>
   <si>
@@ -596,16 +617,28 @@
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode50</t>
   </si>
   <si>
+    <t>String</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode51</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode52</t>
   </si>
   <si>
+    <t>Decimal</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode53</t>
   </si>
   <si>
+    <t>Lei</t>
+  </si>
+  <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode54</t>
+  </si>
+  <si>
+    <t>Isin</t>
   </si>
   <si>
     <t>http://uri.suomi.fi/codelist/test/600/code/testcode55</t>
@@ -656,14 +689,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -715,99 +751,99 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>44</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
         <v>57</v>
@@ -819,16 +855,16 @@
         <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1834,98 +1870,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2936,218 +2972,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -3155,34 +3191,34 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>75</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
         <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -3190,34 +3226,34 @@
         <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
         <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -3225,34 +3261,34 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
         <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -3260,34 +3296,34 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
         <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M10" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -3295,34 +3331,34 @@
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
         <v>88</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -3330,34 +3366,34 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
         <v>91</v>
       </c>
       <c r="I12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M12" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -3365,34 +3401,34 @@
         <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
         <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -3400,34 +3436,34 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H14" t="s">
         <v>97</v>
       </c>
       <c r="I14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -3435,34 +3471,34 @@
         <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
         <v>100</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -3470,34 +3506,34 @@
         <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H16" t="s">
         <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M16" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -3505,34 +3541,34 @@
         <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
         <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H17" t="s">
         <v>106</v>
       </c>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -3540,34 +3576,34 @@
         <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
         <v>108</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
         <v>109</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M18" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -3575,34 +3611,34 @@
         <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
         <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H19" t="s">
         <v>112</v>
       </c>
       <c r="I19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -3610,34 +3646,34 @@
         <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
         <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H20" t="s">
         <v>115</v>
       </c>
       <c r="I20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M20" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -3645,34 +3681,34 @@
         <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
         <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
         <v>118</v>
       </c>
       <c r="I21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M21" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -3680,34 +3716,34 @@
         <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
         <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
         <v>121</v>
       </c>
       <c r="I22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M22" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -3715,34 +3751,34 @@
         <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
         <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H23" t="s">
         <v>124</v>
       </c>
       <c r="I23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -3750,34 +3786,34 @@
         <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
         <v>126</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
         <v>127</v>
       </c>
       <c r="I24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M24" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -3785,34 +3821,34 @@
         <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
         <v>129</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H25" t="s">
         <v>130</v>
       </c>
       <c r="I25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M25" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -3820,34 +3856,34 @@
         <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
         <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H26" t="s">
         <v>133</v>
       </c>
       <c r="I26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M26" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -3855,34 +3891,34 @@
         <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
         <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H27" t="s">
         <v>136</v>
       </c>
       <c r="I27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M27" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -3890,34 +3926,34 @@
         <v>137</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
         <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H28" t="s">
         <v>139</v>
       </c>
       <c r="I28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M28" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -3925,34 +3961,34 @@
         <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
         <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H29" t="s">
         <v>142</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M29" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -3960,34 +3996,34 @@
         <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
         <v>144</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H30" t="s">
         <v>145</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M30" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -3995,34 +4031,34 @@
         <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
         <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H31" t="s">
         <v>148</v>
       </c>
       <c r="I31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="M31" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
@@ -5027,66 +5063,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6088,8 +6124,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.29"/>
-    <col customWidth="1" min="2" max="2" width="12.14"/>
-    <col customWidth="1" min="3" max="3" width="12.57"/>
+    <col customWidth="1" min="2" max="2" width="20.14"/>
+    <col customWidth="1" min="3" max="3" width="22.43"/>
     <col customWidth="1" min="4" max="4" width="18.14"/>
     <col customWidth="1" min="5" max="5" width="20.71"/>
     <col customWidth="1" min="6" max="6" width="51.71"/>
@@ -6114,34 +6150,34 @@
       <c r="D1" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>165</v>
+      <c r="A2" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B2" t="s">
         <v>166</v>
@@ -6149,28 +6185,28 @@
       <c r="C2" t="s">
         <v>167</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F2" t="s">
         <v>170</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="2">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3">
         <v>43101.0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>43831.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>165</v>
+      <c r="A3" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>166</v>
@@ -6178,25 +6214,25 @@
       <c r="C3" t="s">
         <v>167</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F3" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>43102.0</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>43832.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>165</v>
+      <c r="A4" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B4" t="s">
         <v>166</v>
@@ -6204,25 +6240,25 @@
       <c r="C4" t="s">
         <v>167</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F4" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>43103.0</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>43833.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>165</v>
+      <c r="A5" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>166</v>
@@ -6230,25 +6266,25 @@
       <c r="C5" t="s">
         <v>167</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F5" t="s">
         <v>173</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>43104.0</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>43834.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>165</v>
+      <c r="A6" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B6" t="s">
         <v>166</v>
@@ -6256,25 +6292,25 @@
       <c r="C6" t="s">
         <v>167</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F6" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>43105.0</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>43835.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>165</v>
+      <c r="A7" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B7" t="s">
         <v>166</v>
@@ -6282,25 +6318,25 @@
       <c r="C7" t="s">
         <v>167</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F7" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>43106.0</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>43836.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>165</v>
+      <c r="A8" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B8" t="s">
         <v>166</v>
@@ -6308,25 +6344,25 @@
       <c r="C8" t="s">
         <v>167</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E8" t="s">
-        <v>169</v>
+      <c r="E8" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F8" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="2">
+        <v>177</v>
+      </c>
+      <c r="H8" s="3">
         <v>43107.0</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <v>43837.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>165</v>
+      <c r="A9" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B9" t="s">
         <v>166</v>
@@ -6334,25 +6370,25 @@
       <c r="C9" t="s">
         <v>167</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E9" t="s">
-        <v>169</v>
+      <c r="E9" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H9" s="2">
+        <v>178</v>
+      </c>
+      <c r="H9" s="3">
         <v>43108.0</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>43838.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>165</v>
+      <c r="A10" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B10" t="s">
         <v>166</v>
@@ -6360,25 +6396,25 @@
       <c r="C10" t="s">
         <v>167</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E10" t="s">
-        <v>169</v>
+      <c r="E10" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
-      </c>
-      <c r="H10" s="2">
+        <v>179</v>
+      </c>
+      <c r="H10" s="3">
         <v>43109.0</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>43839.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>165</v>
+      <c r="A11" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B11" t="s">
         <v>166</v>
@@ -6386,25 +6422,25 @@
       <c r="C11" t="s">
         <v>167</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E11" t="s">
-        <v>169</v>
+      <c r="E11" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F11" t="s">
-        <v>179</v>
-      </c>
-      <c r="H11" s="2">
+        <v>180</v>
+      </c>
+      <c r="H11" s="3">
         <v>43110.0</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>43840.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>165</v>
+      <c r="A12" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B12" t="s">
         <v>166</v>
@@ -6412,25 +6448,25 @@
       <c r="C12" t="s">
         <v>167</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E12" t="s">
-        <v>169</v>
+      <c r="E12" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F12" t="s">
-        <v>180</v>
-      </c>
-      <c r="H12" s="2">
+        <v>181</v>
+      </c>
+      <c r="H12" s="3">
         <v>43111.0</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <v>43841.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>165</v>
+      <c r="A13" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B13" t="s">
         <v>166</v>
@@ -6438,25 +6474,25 @@
       <c r="C13" t="s">
         <v>167</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E13" t="s">
-        <v>169</v>
+      <c r="E13" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
-      </c>
-      <c r="H13" s="2">
+        <v>183</v>
+      </c>
+      <c r="H13" s="3">
         <v>43112.0</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <v>43842.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>165</v>
+      <c r="A14" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B14" t="s">
         <v>166</v>
@@ -6464,25 +6500,25 @@
       <c r="C14" t="s">
         <v>167</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E14" t="s">
-        <v>169</v>
+      <c r="E14" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
-      </c>
-      <c r="H14" s="2">
+        <v>184</v>
+      </c>
+      <c r="H14" s="3">
         <v>43113.0</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
         <v>43843.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>165</v>
+      <c r="A15" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B15" t="s">
         <v>166</v>
@@ -6490,25 +6526,25 @@
       <c r="C15" t="s">
         <v>167</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E15" t="s">
-        <v>169</v>
+      <c r="E15" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
-      </c>
-      <c r="H15" s="2">
+        <v>186</v>
+      </c>
+      <c r="H15" s="3">
         <v>43114.0</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="3">
         <v>43844.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>165</v>
+      <c r="A16" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="B16" t="s">
         <v>166</v>
@@ -6516,25 +6552,25 @@
       <c r="C16" t="s">
         <v>167</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E16" t="s">
-        <v>169</v>
+      <c r="E16" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
-      </c>
-      <c r="H16" s="2">
+        <v>187</v>
+      </c>
+      <c r="H16" s="3">
         <v>43115.0</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3">
         <v>43845.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>165</v>
+      <c r="A17" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B17" t="s">
         <v>166</v>
@@ -6542,25 +6578,25 @@
       <c r="C17" t="s">
         <v>167</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E17" t="s">
-        <v>169</v>
+      <c r="E17" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
-      </c>
-      <c r="H17" s="2">
+        <v>189</v>
+      </c>
+      <c r="H17" s="3">
         <v>43116.0</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="3">
         <v>43846.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>165</v>
+      <c r="A18" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B18" t="s">
         <v>166</v>
@@ -6568,25 +6604,25 @@
       <c r="C18" t="s">
         <v>167</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E18" t="s">
-        <v>169</v>
+      <c r="E18" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" s="2">
+        <v>190</v>
+      </c>
+      <c r="H18" s="3">
         <v>43117.0</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="3">
         <v>43847.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>165</v>
+      <c r="A19" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B19" t="s">
         <v>166</v>
@@ -6594,25 +6630,25 @@
       <c r="C19" t="s">
         <v>167</v>
       </c>
-      <c r="D19" t="s">
-        <v>168</v>
-      </c>
-      <c r="E19" t="s">
-        <v>169</v>
+      <c r="D19" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F19" t="s">
-        <v>187</v>
-      </c>
-      <c r="H19" s="2">
+        <v>193</v>
+      </c>
+      <c r="H19" s="3">
         <v>43118.0</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="3">
         <v>43848.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>165</v>
+      <c r="A20" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B20" t="s">
         <v>166</v>
@@ -6620,25 +6656,25 @@
       <c r="C20" t="s">
         <v>167</v>
       </c>
-      <c r="D20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E20" t="s">
-        <v>169</v>
+      <c r="D20" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
-      </c>
-      <c r="H20" s="2">
+        <v>194</v>
+      </c>
+      <c r="H20" s="3">
         <v>43119.0</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3">
         <v>43849.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" t="s">
-        <v>165</v>
+      <c r="A21" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B21" t="s">
         <v>166</v>
@@ -6646,25 +6682,25 @@
       <c r="C21" t="s">
         <v>167</v>
       </c>
-      <c r="D21" t="s">
-        <v>168</v>
-      </c>
-      <c r="E21" t="s">
-        <v>169</v>
+      <c r="D21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
-      </c>
-      <c r="H21" s="2">
+        <v>195</v>
+      </c>
+      <c r="H21" s="3">
         <v>43120.0</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="3">
         <v>43850.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>165</v>
+      <c r="A22" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B22" t="s">
         <v>166</v>
@@ -6672,25 +6708,25 @@
       <c r="C22" t="s">
         <v>167</v>
       </c>
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" t="s">
-        <v>169</v>
+      <c r="D22" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="F22" t="s">
-        <v>190</v>
-      </c>
-      <c r="H22" s="2">
+        <v>197</v>
+      </c>
+      <c r="H22" s="3">
         <v>43121.0</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3">
         <v>43851.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" t="s">
-        <v>165</v>
+      <c r="A23" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B23" t="s">
         <v>166</v>
@@ -6698,25 +6734,25 @@
       <c r="C23" t="s">
         <v>167</v>
       </c>
-      <c r="D23" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" t="s">
-        <v>169</v>
+      <c r="D23" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="F23" t="s">
-        <v>191</v>
-      </c>
-      <c r="H23" s="2">
+        <v>198</v>
+      </c>
+      <c r="H23" s="3">
         <v>43122.0</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
         <v>43852.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" t="s">
-        <v>165</v>
+      <c r="A24" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B24" t="s">
         <v>166</v>
@@ -6724,25 +6760,25 @@
       <c r="C24" t="s">
         <v>167</v>
       </c>
-      <c r="D24" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" t="s">
-        <v>169</v>
+      <c r="D24" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
-      </c>
-      <c r="H24" s="2">
+        <v>199</v>
+      </c>
+      <c r="H24" s="3">
         <v>43123.0</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
         <v>43853.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" t="s">
-        <v>165</v>
+      <c r="A25" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B25" t="s">
         <v>166</v>
@@ -6750,25 +6786,25 @@
       <c r="C25" t="s">
         <v>167</v>
       </c>
-      <c r="D25" t="s">
-        <v>168</v>
-      </c>
-      <c r="E25" t="s">
-        <v>169</v>
+      <c r="D25" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
-      </c>
-      <c r="H25" s="2">
+        <v>201</v>
+      </c>
+      <c r="H25" s="3">
         <v>43124.0</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
         <v>43854.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" t="s">
-        <v>165</v>
+      <c r="A26" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B26" t="s">
         <v>166</v>
@@ -6776,25 +6812,25 @@
       <c r="C26" t="s">
         <v>167</v>
       </c>
-      <c r="D26" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" t="s">
-        <v>169</v>
+      <c r="D26" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="F26" t="s">
-        <v>194</v>
-      </c>
-      <c r="H26" s="2">
+        <v>202</v>
+      </c>
+      <c r="H26" s="3">
         <v>43125.0</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
         <v>43855.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" t="s">
-        <v>165</v>
+      <c r="A27" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B27" t="s">
         <v>166</v>
@@ -6802,25 +6838,25 @@
       <c r="C27" t="s">
         <v>167</v>
       </c>
-      <c r="D27" t="s">
-        <v>168</v>
-      </c>
-      <c r="E27" t="s">
-        <v>169</v>
+      <c r="D27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="F27" t="s">
-        <v>195</v>
-      </c>
-      <c r="H27" s="2">
+        <v>204</v>
+      </c>
+      <c r="H27" s="3">
         <v>43126.0</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <v>43856.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" t="s">
-        <v>165</v>
+      <c r="A28" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B28" t="s">
         <v>166</v>
@@ -6828,25 +6864,25 @@
       <c r="C28" t="s">
         <v>167</v>
       </c>
-      <c r="D28" t="s">
-        <v>168</v>
-      </c>
-      <c r="E28" t="s">
-        <v>169</v>
+      <c r="D28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="F28" t="s">
-        <v>196</v>
-      </c>
-      <c r="H28" s="2">
+        <v>206</v>
+      </c>
+      <c r="H28" s="3">
         <v>43127.0</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
         <v>43857.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" t="s">
-        <v>165</v>
+      <c r="A29" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B29" t="s">
         <v>166</v>
@@ -6854,25 +6890,25 @@
       <c r="C29" t="s">
         <v>167</v>
       </c>
-      <c r="D29" t="s">
-        <v>168</v>
-      </c>
-      <c r="E29" t="s">
-        <v>169</v>
+      <c r="D29" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="F29" t="s">
-        <v>197</v>
-      </c>
-      <c r="H29" s="2">
+        <v>208</v>
+      </c>
+      <c r="H29" s="3">
         <v>43128.0</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <v>43858.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" t="s">
-        <v>165</v>
+      <c r="A30" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B30" t="s">
         <v>166</v>
@@ -6880,25 +6916,25 @@
       <c r="C30" t="s">
         <v>167</v>
       </c>
-      <c r="D30" t="s">
-        <v>168</v>
-      </c>
-      <c r="E30" t="s">
-        <v>169</v>
+      <c r="D30" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="F30" t="s">
-        <v>198</v>
-      </c>
-      <c r="H30" s="2">
+        <v>209</v>
+      </c>
+      <c r="H30" s="3">
         <v>43129.0</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
         <v>43859.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" t="s">
-        <v>165</v>
+      <c r="A31" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="B31" t="s">
         <v>166</v>
@@ -6906,19 +6942,19 @@
       <c r="C31" t="s">
         <v>167</v>
       </c>
-      <c r="D31" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" t="s">
-        <v>169</v>
+      <c r="D31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="F31" t="s">
-        <v>199</v>
-      </c>
-      <c r="H31" s="2">
+        <v>210</v>
+      </c>
+      <c r="H31" s="3">
         <v>43130.0</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
         <v>43860.0</v>
       </c>
     </row>

</xml_diff>